<commit_message>
Added stocks for week 2
</commit_message>
<xml_diff>
--- a/Start Your Own/position_sizing_calculator_with_summary.xlsx
+++ b/Start Your Own/position_sizing_calculator_with_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oferg/work/mycode/ChatGPT-Micro-Cap-Experiment/Start Your Own/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603A7F6B-83D6-A047-94A0-8756F2DDD70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E51D7E-74FD-6646-91D5-842421985147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="31300" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,13 +87,13 @@
     <t>PVLV</t>
   </si>
   <si>
-    <t>CNXC</t>
-  </si>
-  <si>
-    <t>Max Risk per Trade (10%) ($)</t>
-  </si>
-  <si>
-    <t>Real risk</t>
+    <t>Real risk (%)</t>
+  </si>
+  <si>
+    <t>MAX_RSIK</t>
+  </si>
+  <si>
+    <t>XLF</t>
   </si>
 </sst>
 </file>
@@ -433,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:K5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -473,10 +473,11 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="H1" t="str">
+        <f>"Max Risk per Trade (" &amp; B23*100 &amp; "%) ($)"</f>
+        <v>Max Risk per Trade (10%) ($)</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -514,7 +515,7 @@
         <v>7.9999999999999973</v>
       </c>
       <c r="H2">
-        <f>B2*0.1</f>
+        <f>B2*$B$23</f>
         <v>15</v>
       </c>
       <c r="I2">
@@ -556,7 +557,7 @@
         <v>7.9999999999999929</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H5" si="3">B3*0.1</f>
+        <f t="shared" ref="H3:H10" si="3">B3*$B$23</f>
         <v>15</v>
       </c>
       <c r="I3">
@@ -616,40 +617,40 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5">
-        <v>438</v>
+        <v>380</v>
       </c>
       <c r="C5">
-        <v>54.81</v>
+        <v>54.32</v>
       </c>
       <c r="D5">
         <v>8</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>50.425200000000004</v>
+        <v>49.974400000000003</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>4.3847999999999985</v>
+        <v>4.3455999999999975</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>7.9999999999999964</v>
+        <v>7.9999999999999947</v>
       </c>
       <c r="H5">
         <f t="shared" si="3"/>
-        <v>43.800000000000004</v>
+        <v>38</v>
       </c>
       <c r="I5">
         <f t="shared" si="4"/>
-        <v>7.9912424740010941</v>
+        <v>6.9955817378497791</v>
       </c>
       <c r="J5">
         <f t="shared" si="5"/>
-        <v>438</v>
+        <v>380</v>
       </c>
       <c r="K5">
         <f t="shared" si="6"/>
@@ -670,11 +671,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H6">
-        <f>B6*0.02</f>
+        <f>B6*$B$23</f>
         <v>0</v>
       </c>
       <c r="I6" t="e">
-        <f t="shared" ref="I3:I11" si="7">MIN(INT(H6/F6), INT(B6/C6))</f>
+        <f t="shared" ref="I6:I11" si="7">MIN(INT(H6/F6), INT(B6/C6))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J6" t="e">
@@ -700,7 +701,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H7">
-        <f>B7*0.02</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I7" t="e">
@@ -730,7 +731,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H8">
-        <f>B8*0.02</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I8" t="e">
@@ -760,7 +761,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H9">
-        <f>B9*0.02</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I9" t="e">
@@ -790,7 +791,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H10">
-        <f>B10*0.02</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I10" t="e">
@@ -812,7 +813,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <f>B11*0.02</f>
+        <f t="shared" ref="H11" si="8">B11*0.02</f>
         <v>0</v>
       </c>
       <c r="I11" t="e">
@@ -868,6 +869,16 @@
       <c r="K16">
         <f t="shared" si="6"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>